<commit_message>
Replaced filenames for trials
</commit_message>
<xml_diff>
--- a/html/resources/trainingtrials_social_prob.xlsx
+++ b/html/resources/trainingtrials_social_prob.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raimundbuehler/Documents/UNIDOCS/RALTfinal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raimundbuehler/Desktop/RALT_PLD_english/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29840C69-5569-1B4D-A6F4-B9995FDD06DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C47484B-CE86-1246-8AD6-DEFFC847B29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9820" yWindow="1840" windowWidth="26740" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Stim</t>
   </si>
@@ -43,43 +43,22 @@
     <t>B</t>
   </si>
   <si>
-    <t>ADFES/Freigestellt/Neutral/F04-Neutral-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Joy/Used/F04-Joy-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Anger/F04-Anger-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Neutral/M02-Neutral-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Joy/Used/M02-Joy-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Anger/M02-Anger-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Neutral/F01-Neutral-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Joy/Used/F01-Joy-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Anger/F01-Anger-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Neutral/M06-Neutral-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Joy/Used/M06-Joy-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
-    <t>ADFES/Freigestellt/Anger/M06-Anger-Face Forward_freigestellt.mp4</t>
-  </si>
-  <si>
     <t>CorrCatProb</t>
+  </si>
+  <si>
+    <t>Stimuli/neutral/Still.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/social/happy/F01-Happy Women.mp4</t>
+  </si>
+  <si>
+    <t>Stimuli/social/angry/F04-Angry Women.mp4</t>
+  </si>
+  <si>
+    <t>Stimuli/social/happy/M02-Happy Man.mp4</t>
+  </si>
+  <si>
+    <t>Stimuli/social/angry/M06-Angry Man.mp4</t>
   </si>
 </sst>
 </file>
@@ -451,7 +430,7 @@
   <dimension ref="A1:V91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,7 +452,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -481,13 +460,13 @@
         <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -499,7 +478,7 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -516,13 +495,13 @@
         <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -534,13 +513,13 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>

</xml_diff>